<commit_message>
Working on TTA config. Non inverted rescue.
</commit_message>
<xml_diff>
--- a/Tiny talon/M1 Pitch calcs.xlsx
+++ b/Tiny talon/M1 Pitch calcs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Phils Projects\rotorflight\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Phils Projects\Heli-config\rotorflight-config\Tiny talon\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -371,11 +371,11 @@
         <v>125</v>
       </c>
       <c r="D2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E2">
         <f>DEGREES(ASIN((D2/2)/C2))</f>
-        <v>11.53695903281549</v>
+        <v>9.2068962213459002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>